<commit_message>
Added correct data JFree Chart
</commit_message>
<xml_diff>
--- a/Corelation Data Analysis/Jfree Chart/Corelation Result.xlsx
+++ b/Corelation Data Analysis/Jfree Chart/Corelation Result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikunj\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karansharma/Desktop/untitled folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149D2028-7DCF-4D81-AA82-369E35243516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4784031F-FBB4-2C4C-BB49-80FAE1466473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{18BB63F1-A364-F74A-BAEB-0C1A9B26E513}"/>
+    <workbookView xWindow="1880" yWindow="3480" windowWidth="28040" windowHeight="16020" xr2:uid="{18BB63F1-A364-F74A-BAEB-0C1A9B26E513}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,6 +41,21 @@
     <t>Spearman Coefficient</t>
   </si>
   <si>
+    <t>Metrics 1-3  Jacoco version 1.0.19</t>
+  </si>
+  <si>
+    <t>Metrics 1-4  Jacoco version 1.0.19</t>
+  </si>
+  <si>
+    <t>Metrics  2-4  Jacoco version 1.0.19</t>
+  </si>
+  <si>
+    <t>Metrics 2-3  Jacoco version 1.0.19</t>
+  </si>
+  <si>
+    <t>Metrics  5-6  Jacoco version 1.0.19</t>
+  </si>
+  <si>
     <t>Metrics 1-6  Jfree Chart 1.0.14,1.0.15,1.0.16,1.0.17,1.0.18,1.0.19</t>
   </si>
   <si>
@@ -52,21 +69,6 @@
   </si>
   <si>
     <t>Class Level</t>
-  </si>
-  <si>
-    <t>Metrics 1-4   version 1.0.19</t>
-  </si>
-  <si>
-    <t>Metrics  2-4   version 1.0.19</t>
-  </si>
-  <si>
-    <t>Metrics 1-3   version 1.0.19</t>
-  </si>
-  <si>
-    <t>Metrics 2-3   version 1.0.19</t>
-  </si>
-  <si>
-    <t>Metrics  5-6   version 1.0.19</t>
   </si>
 </sst>
 </file>
@@ -82,26 +84,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,9 +125,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,124 +442,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA4C7678-4ACC-6242-A974-4E5E09C58F19}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="58" customWidth="1"/>
-    <col min="2" max="2" width="57.125" customWidth="1"/>
-    <col min="3" max="3" width="28.5" customWidth="1"/>
+    <col min="1" max="1" width="58" style="2" customWidth="1"/>
+    <col min="2" max="2" width="57.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.5" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.95138791445583903</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.94516414444873198</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.93476355388580501</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.61341232088798803</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2">
         <v>0.84179235354436199</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2.4686956694861501E-2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.77145286098992305</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>-0.98262379836822999</v>
       </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>-0.78262379212492605</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2">
         <v>-1</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>